<commit_message>
Changes readme and graph
</commit_message>
<xml_diff>
--- a/docs/results.xlsx
+++ b/docs/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\u\usr\pro\2022_biclean\MTEvalPoC\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A990B2F-0C6C-4E9B-8510-DE9AFB15BD11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1015618B-06B7-4153-81AB-A99C6F37A5C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1110" yWindow="-120" windowWidth="27810" windowHeight="16440" xr2:uid="{52D6FD14-6F51-4F1A-A4DC-179A69883456}"/>
+    <workbookView xWindow="1950" yWindow="0" windowWidth="26175" windowHeight="16200" xr2:uid="{52D6FD14-6F51-4F1A-A4DC-179A69883456}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -1952,13 +1952,19 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Hoja1!$F$31:$F$32</c:f>
+              <c:f>Hoja1!$F$29:$F$32</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
+                  <c:v>GOLD</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>WATSON</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>DEEPL</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
                   <c:v>GOOGLE</c:v>
                 </c:pt>
               </c:strCache>
@@ -1966,14 +1972,20 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$G$31:$G$32</c:f>
+              <c:f>Hoja1!$G$29:$G$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
+                  <c:v>0.82777838732537801</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.83104474938427098</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>0.82287625604915804</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
                   <c:v>0.84219848374578898</c:v>
                 </c:pt>
               </c:numCache>
@@ -1981,7 +1993,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-9BAB-47A1-884C-E288AC3F0858}"/>
+              <c16:uniqueId val="{00000000-E97C-4CF6-BB1F-064C3B8C1F7F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1995,11 +2007,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="187117071"/>
-        <c:axId val="663860495"/>
+        <c:axId val="93877968"/>
+        <c:axId val="94343776"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="187117071"/>
+        <c:axId val="93877968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2042,7 +2054,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="663860495"/>
+        <c:crossAx val="94343776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2050,7 +2062,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="663860495"/>
+        <c:axId val="94343776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2101,7 +2113,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="187117071"/>
+        <c:crossAx val="93877968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6171,23 +6183,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1557337</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>72</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>423862</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Gráfico 5">
+        <xdr:cNvPr id="7" name="Gráfico 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C05DDF9B-5AAA-6682-912E-4860D4A77C6E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{295EF7A6-DAB7-B987-EF96-56C7971ABF1E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6507,8 +6519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD330BFB-C417-49B1-A343-06FE9B49C000}">
   <dimension ref="A1:H70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28:G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>